<commit_message>
reformatting Pt Cloates dataset
</commit_message>
<xml_diff>
--- a/outputs/PtCloates/PtCloatesBOSS_fishlist_GC.xlsx
+++ b/outputs/PtCloates/PtCloatesBOSS_fishlist_GC.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10522231\MEG\GC_Chapter3_BRUVSvsDropCam\outputs\PtCloates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF012367-06E7-4083-9786-2754BF24FD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01540B2B-1385-42C8-90C0-46834F93A877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32340" yWindow="180" windowWidth="18036" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PtCloatesBOSS_fishlist" sheetId="1" r:id="rId1"/>
     <sheet name="minus_Sus_sus" sheetId="2" r:id="rId2"/>
     <sheet name="minus_Unknown_Genus" sheetId="3" r:id="rId3"/>
+    <sheet name="plus_Unknown_Genus" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="139">
   <si>
     <t>family</t>
   </si>
@@ -424,6 +425,21 @@
   </si>
   <si>
     <t>too far away to tell, leave as spp</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change to fasciata </t>
+  </si>
+  <si>
+    <t>YES processed on BOSS emobs.</t>
+  </si>
+  <si>
+    <t>RE-EXPORTED 2022 NAKED DONE</t>
+  </si>
+  <si>
+    <t>RE-EXPORTED 2021 BOSS DONE</t>
   </si>
 </sst>
 </file>
@@ -2535,8 +2551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3755,10 +3771,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M60"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection sqref="A1:E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3766,6 +3782,7 @@
     <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -4038,6 +4055,9 @@
       <c r="I14" t="s">
         <v>130</v>
       </c>
+      <c r="K14" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -4058,6 +4078,9 @@
       <c r="G15" t="s">
         <v>122</v>
       </c>
+      <c r="K15" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -4361,7 +4384,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -4378,7 +4401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -4395,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>62</v>
       </c>
@@ -4412,7 +4435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -4429,7 +4452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -4446,7 +4469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -4463,7 +4486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -4485,8 +4508,11 @@
       <c r="I39" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -4504,7 +4530,7 @@
       </c>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -4521,7 +4547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -4538,7 +4564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -4555,7 +4581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>83</v>
       </c>
@@ -4572,7 +4598,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -4589,7 +4615,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -4606,7 +4632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -4623,7 +4649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -4813,6 +4839,15 @@
       <c r="G58" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="I58" t="s">
+        <v>135</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="M58" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
@@ -4833,8 +4868,11 @@
       <c r="G59" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="M59" t="s">
-        <v>112</v>
+      <c r="I59" t="s">
+        <v>125</v>
+      </c>
+      <c r="K59" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
@@ -4858,6 +4896,1241 @@
       </c>
       <c r="I60" t="s">
         <v>118</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K64" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K65" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2174B48F-1A5C-43B8-9EFA-CF3E59EFF537}">
+  <dimension ref="A1:E71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51">
+        <v>8</v>
+      </c>
+      <c r="E51">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54">
+        <v>31</v>
+      </c>
+      <c r="E54">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59">
+        <v>4</v>
+      </c>
+      <c r="E59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>104</v>
+      </c>
+      <c r="B61" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="E61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>104</v>
+      </c>
+      <c r="B62" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" t="s">
+        <v>108</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>104</v>
+      </c>
+      <c r="B65" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" t="s">
+        <v>111</v>
+      </c>
+      <c r="C66" t="s">
+        <v>112</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" t="s">
+        <v>113</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>104</v>
+      </c>
+      <c r="B68" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68">
+        <v>4</v>
+      </c>
+      <c r="E68">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>104</v>
+      </c>
+      <c r="B69" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>114</v>
+      </c>
+      <c r="B70" t="s">
+        <v>115</v>
+      </c>
+      <c r="C70" t="s">
+        <v>120</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>